<commit_message>
Updated Deployment utility to allow mutiple variables.
</commit_message>
<xml_diff>
--- a/APS to SQL DW Migration - Schema and Data Migration with PolyBase/APS migration(Customer)  - Questionnaire.xlsx
+++ b/APS to SQL DW Migration - Schema and Data Migration with PolyBase/APS migration(Customer)  - Questionnaire.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/charis_microsoft_com/Documents/Clients/Azure DW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charis\OneDrive - Microsoft\GitHubForMS\AzureDWScriptsandUtilities\APS to SQL DW Migration - Schema and Data Migration with PolyBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="0B698C7034354603A8321A596B4C7E502CE0125B" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{8EA1430E-937C-48A3-8897-1BAC962EDD4D}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="0B698C7034354603A8321A596B4C7E502CE0125B" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{7F86AF2D-96C3-4CD2-8945-E993B3542C76}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="9353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current APS Environment - Cust" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -32,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
-    <t>APS Questionnaire</t>
-  </si>
-  <si>
     <t>Hardware Features</t>
   </si>
   <si>
@@ -44,15 +36,6 @@
     <t>Answers</t>
   </si>
   <si>
-    <t>How many scale units of PDW?</t>
-  </si>
-  <si>
-    <t>How many scale units of HDI?</t>
-  </si>
-  <si>
-    <t>Is there a Loading Server?  If so, is it connected via Infiniband?</t>
-  </si>
-  <si>
     <t>How much storage is available(Free Space) on the loading Server?</t>
   </si>
   <si>
@@ -288,13 +271,25 @@
   </si>
   <si>
     <t>Is there test data available to be used during migration and testing?</t>
+  </si>
+  <si>
+    <t>MPP Questionnaire</t>
+  </si>
+  <si>
+    <t>Make and Model of your Appliance for each Environment? (CPUs, GPUs, memory)</t>
+  </si>
+  <si>
+    <t>List the storage space, Memory, Cores and/or FGPAs for each environment?</t>
+  </si>
+  <si>
+    <t>Is there a Loading Server?  If so, is it connected to the Appliance?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,638 +738,638 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.73046875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="8"/>
       <c r="B1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="2"/>
       <c r="B8" s="5"/>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:3" ht="28.9">
+    <row r="15" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="B16" s="5"/>
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A17" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" ht="15.75">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" ht="28.9">
+    <row r="22" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A25" s="2"/>
       <c r="B25" s="5"/>
       <c r="C25" s="11"/>
     </row>
-    <row r="26" spans="1:3" ht="28.15">
+    <row r="26" spans="1:3" ht="28.15" x14ac:dyDescent="0.5">
       <c r="A26" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C27" s="10"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C29" s="10"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C30" s="10"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31" s="10"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C32" s="10"/>
     </row>
-    <row r="33" spans="1:3" ht="15.75">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C33" s="10"/>
     </row>
-    <row r="34" spans="1:3" ht="28.9">
+    <row r="34" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="10"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C35" s="10"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="1:3" ht="28.15">
+    <row r="37" spans="1:3" ht="28.15" x14ac:dyDescent="0.5">
       <c r="A37" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C37" s="10"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" ht="28.9">
+    <row r="39" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A40" s="3"/>
       <c r="B40" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:3" ht="28.9">
+    <row r="43" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:3" ht="28.9">
+    <row r="44" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" ht="28.9">
+    <row r="45" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75">
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A46" s="2"/>
       <c r="B46" s="5"/>
       <c r="C46" s="11"/>
     </row>
-    <row r="47" spans="1:3" ht="28.15">
+    <row r="47" spans="1:3" ht="28.15" x14ac:dyDescent="0.5">
       <c r="A47" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75">
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75">
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A49" s="3"/>
       <c r="B49" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75">
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75">
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75">
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" ht="15.75">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A53" s="3"/>
       <c r="B53" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" ht="15.75">
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A55" s="3"/>
       <c r="B55" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C55" s="10"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75">
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A56" s="3"/>
       <c r="B56" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C56" s="10"/>
     </row>
-    <row r="57" spans="1:3" ht="28.9">
+    <row r="57" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C57" s="10"/>
     </row>
-    <row r="58" spans="1:3" ht="15.75">
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="3"/>
       <c r="B58" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C58" s="10"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75">
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A59" s="3"/>
       <c r="B59" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C59" s="10"/>
     </row>
-    <row r="60" spans="1:3" ht="15.75">
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C60" s="10"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75">
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A61" s="3"/>
       <c r="B61" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C61" s="10"/>
     </row>
-    <row r="62" spans="1:3" ht="15.75">
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A62" s="2"/>
       <c r="B62" s="5"/>
       <c r="C62" s="11"/>
     </row>
-    <row r="63" spans="1:3" ht="15.75">
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A63" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C63" s="10"/>
     </row>
-    <row r="64" spans="1:3" ht="15.75">
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A64" s="3"/>
       <c r="B64" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C64" s="10"/>
     </row>
-    <row r="65" spans="1:3" ht="15.75">
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A65" s="3"/>
       <c r="B65" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C65" s="10"/>
     </row>
-    <row r="66" spans="1:3" ht="15.75">
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A66" s="2"/>
       <c r="B66" s="5"/>
       <c r="C66" s="11"/>
     </row>
-    <row r="67" spans="1:3" ht="15.75">
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A67" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C67" s="10"/>
     </row>
-    <row r="68" spans="1:3" ht="15.75">
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A68" s="3"/>
       <c r="B68" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C68" s="10"/>
     </row>
-    <row r="69" spans="1:3" ht="15.75">
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A69" s="3"/>
       <c r="B69" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C69" s="10"/>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A70" s="3"/>
       <c r="B70" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C70" s="10"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75">
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="3"/>
       <c r="B71" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C71" s="10"/>
     </row>
-    <row r="72" spans="1:3" ht="15.75">
+    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:3" ht="15.75">
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A73" s="3"/>
       <c r="C73" s="10"/>
     </row>
-    <row r="74" spans="1:3" ht="15.75">
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="2"/>
       <c r="B74" s="5"/>
       <c r="C74" s="11"/>
     </row>
-    <row r="75" spans="1:3" ht="28.15">
+    <row r="75" spans="1:3" ht="28.15" x14ac:dyDescent="0.5">
       <c r="A75" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C75" s="10"/>
     </row>
-    <row r="76" spans="1:3" ht="15.75">
+    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A76" s="3"/>
       <c r="B76" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C76" s="10"/>
     </row>
-    <row r="77" spans="1:3" ht="15.75">
+    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A77" s="3"/>
       <c r="B77" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C77" s="10"/>
     </row>
-    <row r="78" spans="1:3" ht="28.9">
+    <row r="78" spans="1:3" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A78" s="3"/>
       <c r="B78" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C78" s="10"/>
     </row>
-    <row r="79" spans="1:3" ht="15.75">
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="2"/>
       <c r="B79" s="5"/>
       <c r="C79" s="11"/>
     </row>
-    <row r="80" spans="1:3" ht="28.15">
+    <row r="80" spans="1:3" ht="28.15" x14ac:dyDescent="0.5">
       <c r="A80" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C80" s="10"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75">
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C81" s="10"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="3"/>
       <c r="B82" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A83" s="2"/>
       <c r="B83" s="5"/>
       <c r="C83" s="11"/>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="3"/>
       <c r="B85" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" s="3"/>
       <c r="B86" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="3"/>
       <c r="B87" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="3"/>
       <c r="B88" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="3"/>
       <c r="B89" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="3"/>
       <c r="B90" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A91" s="2"/>
       <c r="B91" s="5"/>
       <c r="C91" s="11"/>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="3"/>
       <c r="B93" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="3"/>
       <c r="B94" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="3"/>
       <c r="B95" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1387,6 +1382,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100690242BDE30F014F83329AA536B70806" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b574e4e36304a5d3dc8b869e43a3722f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b018db0b-322c-4925-9fdb-2f34949f0610" xmlns:ns3="738c2dd8-7dd6-440d-aa04-76a8929a2564" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94a415895028a325dd09a0449796a490" ns2:_="" ns3:_="">
     <xsd:import namespace="b018db0b-322c-4925-9fdb-2f34949f0610"/>
@@ -1575,12 +1576,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1591,13 +1586,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FAF7E1A-C178-4342-9747-E1BF9BECFAEA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB2FB8D4-2738-4081-A92F-3A631B2C6297}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="738c2dd8-7dd6-440d-aa04-76a8929a2564"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b018db0b-322c-4925-9fdb-2f34949f0610"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB2FB8D4-2738-4081-A92F-3A631B2C6297}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FAF7E1A-C178-4342-9747-E1BF9BECFAEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b018db0b-322c-4925-9fdb-2f34949f0610"/>
+    <ds:schemaRef ds:uri="738c2dd8-7dd6-440d-aa04-76a8929a2564"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04C15D6B-260A-4EC1-ADBA-658ECC6774BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04C15D6B-260A-4EC1-ADBA-658ECC6774BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>